<commit_message>
Add initial feature selection step
Signed-off-by: Nardus Mollentze <nmollentze@gmail.com>
</commit_message>
<xml_diff>
--- a/data/internal/ace2_accessions.xlsx
+++ b/data/internal/ace2_accessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nardus/Documents/Postdocs/ace2/data/internal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A861B96-230E-6844-9E22-78D232B0FCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D289B7-4EEE-B749-AD4A-6919D31A5703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,7 +687,7 @@
     <t>haddock_species</t>
   </si>
   <si>
-    <t>Canis lupus</t>
+    <t>Canis lupus familiaris</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="61">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1277,146 +1277,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1814,7 +1674,7 @@
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3865,18 +3725,18 @@
     <sortCondition ref="D2:D100"/>
   </sortState>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="duplicateValues" dxfId="67" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="beginsWith" dxfId="66" priority="66" operator="beginsWith" text="NA">
+    <cfRule type="beginsWith" dxfId="59" priority="66" operator="beginsWith" text="NA">
       <formula>LEFT(D1,LEN("NA"))="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="this_species">
+    <cfRule type="containsText" dxfId="58" priority="64" operator="containsText" text="this_species">
       <formula>NOT(ISERROR(SEARCH("this_species",E1)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="64" priority="65">
+    <cfRule type="containsBlanks" dxfId="57" priority="65">
       <formula>LEN(TRIM(E1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Match ACE2 metadata files to avoid duplication
</commit_message>
<xml_diff>
--- a/data/internal/ace2_accessions.xlsx
+++ b/data/internal/ace2_accessions.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Bos taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">NP_001019673.2</t>
+    <t xml:space="preserve">XP_005228485.1</t>
   </si>
   <si>
     <t xml:space="preserve">Bubalus bubalis</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">Felis catus</t>
   </si>
   <si>
-    <t xml:space="preserve">AAX59005.1</t>
+    <t xml:space="preserve">XP_023104564.1</t>
   </si>
   <si>
     <t xml:space="preserve">Lynx canadensis</t>
@@ -1485,19 +1485,20 @@
   </sheetPr>
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.33"/>
   </cols>
   <sheetData>
@@ -1664,7 +1665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>